<commit_message>
excel updated second time
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Githubtesting\SampleGitProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C5C00-6EA9-4D75-A7C7-294728DDAA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D286E-CD2C-45E1-8011-6F637998A1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>test2</t>
   </si>
   <si>
     <t>another commit from demo1 local</t>
+  </si>
+  <si>
+    <t>test11</t>
   </si>
 </sst>
 </file>
@@ -353,25 +353,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel sheet1 test22 and sheet2added
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Githubtesting\SampleGitProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D286E-CD2C-45E1-8011-6F637998A1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD975A2-94BD-483F-AA33-514A12E4966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,15 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>test2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>another commit from demo1 local</t>
   </si>
   <si>
     <t>test11</t>
+  </si>
+  <si>
+    <t>sheet2_t1</t>
+  </si>
+  <si>
+    <t>sheet2_t2</t>
+  </si>
+  <si>
+    <t>test22</t>
   </si>
 </sst>
 </file>
@@ -354,7 +361,37 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FFCDF4-20AA-4C61-A423-DC7A76F6F64B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,12 +403,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>